<commit_message>
Certification Data for Data Analytics, Fixed Storage Url in Environments, Multiple Social Icons, Multiple Profile Photos
</commit_message>
<xml_diff>
--- a/iac/data/xlsx/certification.xlsx
+++ b/iac/data/xlsx/certification.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wheel\WebstormProjects\CloudGuruChallenge_21.04\data\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wheel\WebstormProjects\Resume\iac\data\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAC28F08-42EC-49D6-AE24-8F1835D6103A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF841755-FEA8-4E11-B7D7-580589FAFA45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="74">
   <si>
     <t>level</t>
   </si>
@@ -311,6 +311,21 @@
     <t>[
 "A Cloud Digital Leader can articulate the capabilities of Google Cloud core products and services and how they benefit organizations. The Cloud Digital Leader can also describe common business use cases and how cloud solutions support an enterprise.",
 "The Cloud Digital Leader exam is job-role agnostic and does not require hands-on experience with Google Cloud."
+]</t>
+  </si>
+  <si>
+    <t>ff44f4b1-a3de-40a2-bbfc-2f1d53b60c86</t>
+  </si>
+  <si>
+    <t>Data Analytics Specialty</t>
+  </si>
+  <si>
+    <t>L622V9QJEJ41135K</t>
+  </si>
+  <si>
+    <t>[
+"Ability to define AWS data analytics services and understand how they integrate with each other",
+"Ability to explain how AWS data analytics services fit in the data lifecycle of collection, storage, processing, and visualization"
 ]</t>
   </si>
 </sst>
@@ -1202,10 +1217,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:J1"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1415,28 +1430,28 @@
     </row>
     <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>19</v>
+        <v>71</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>27</v>
+        <v>72</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>45</v>
+        <v>73</v>
       </c>
       <c r="E7" s="5">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F7" s="5">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="G7" s="5">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="H7" s="5">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="I7" s="5" t="s">
         <v>5</v>
@@ -1447,28 +1462,28 @@
     </row>
     <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E8" s="5">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="F8" s="5">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="G8" s="5">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="H8" s="5">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="I8" s="5" t="s">
         <v>5</v>
@@ -1479,31 +1494,31 @@
     </row>
     <row r="9" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E9" s="5">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F9" s="5">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="G9" s="5">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="H9" s="5">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J9" s="5" t="s">
         <v>7</v>
@@ -1511,25 +1526,25 @@
     </row>
     <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E10" s="5">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="F10" s="5">
         <v>2023</v>
       </c>
       <c r="G10" s="5">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="H10" s="5">
         <v>2020</v>
@@ -1543,119 +1558,151 @@
     </row>
     <row r="11" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
+        <v>48</v>
+      </c>
+      <c r="E11" s="5">
+        <v>12</v>
+      </c>
+      <c r="F11" s="5">
+        <v>2023</v>
+      </c>
       <c r="G11" s="5">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="H11" s="5">
         <v>2020</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>66</v>
+        <v>23</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>68</v>
+        <v>31</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="E12" s="5">
-        <v>6</v>
-      </c>
-      <c r="F12" s="5">
-        <v>2024</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
       <c r="G12" s="5">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H12" s="5">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="I12" s="5" t="s">
         <v>3</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>67</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" s="5"/>
+        <v>66</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>68</v>
+      </c>
       <c r="D13" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
+        <v>69</v>
+      </c>
+      <c r="E13" s="5">
+        <v>6</v>
+      </c>
+      <c r="F13" s="5">
+        <v>2024</v>
+      </c>
       <c r="G13" s="5">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="H13" s="5">
-        <v>2016</v>
+        <v>2021</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>9</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="5"/>
+      <c r="D14" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5">
+        <v>10</v>
+      </c>
+      <c r="H14" s="5">
+        <v>2016</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="J14" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B15" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C15" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D15" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E15" s="5">
         <v>9</v>
       </c>
-      <c r="F14" s="5">
+      <c r="F15" s="5">
         <v>2021</v>
       </c>
-      <c r="G14" s="5">
+      <c r="G15" s="5">
         <v>9</v>
       </c>
-      <c r="H14" s="5">
+      <c r="H15" s="5">
         <v>2020</v>
       </c>
-      <c r="I14" s="5" t="s">
+      <c r="I15" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="J14" s="5" t="s">
+      <c r="J15" s="5" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>